<commit_message>
czc xml scheme added
</commit_message>
<xml_diff>
--- a/data/excel/namapovani_poli.xlsx
+++ b/data/excel/namapovani_poli.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Dusan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/681e67afaf0f621d/Počítač/PROJEKTY/helios-xml-exports/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BDE978A5DA6EB953BED180496C8EBB34CFC9BE7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Alza" sheetId="1" r:id="rId1"/>
+    <sheet name="CZC" sheetId="2" r:id="rId2"/>
+    <sheet name="Onlineshop" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>PriceWithFee</t>
   </si>
@@ -96,12 +99,111 @@
   </si>
   <si>
     <t>sklad_helios.xlsx</t>
+  </si>
+  <si>
+    <t>CZC_HELIOS.xml</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>ESHOP_CODE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>EAN</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>MANUFACTURER</t>
+  </si>
+  <si>
+    <t>IMAGE</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>AUTHOR_FEE</t>
+  </si>
+  <si>
+    <t>RECYCLE_FEE</t>
+  </si>
+  <si>
+    <t>WEIGHT_BRUTTO</t>
+  </si>
+  <si>
+    <t>SIZE_X_NETTO</t>
+  </si>
+  <si>
+    <t>SIZE_Y_NETTO</t>
+  </si>
+  <si>
+    <t>SIZE_Z_NETTO</t>
+  </si>
+  <si>
+    <t>WARRANTY</t>
+  </si>
+  <si>
+    <t>Prodejní cena</t>
+  </si>
+  <si>
+    <t>Hmotnost</t>
+  </si>
+  <si>
+    <t>Šířka</t>
+  </si>
+  <si>
+    <t>Výška</t>
+  </si>
+  <si>
+    <t>Hloubka</t>
+  </si>
+  <si>
+    <t>onlineshop.xml</t>
+  </si>
+  <si>
+    <t>ITEM_ID</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>IMGURL</t>
+  </si>
+  <si>
+    <t>PRICE_NAKUP</t>
+  </si>
+  <si>
+    <t>PRICE_DOPORUCENA</t>
+  </si>
+  <si>
+    <t>Cena v HM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,16 +276,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,30 +565,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -521,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -559,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -586,4 +691,254 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added onlineshop option for xml exporting
</commit_message>
<xml_diff>
--- a/data/excel/namapovani_poli.xlsx
+++ b/data/excel/namapovani_poli.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_BDE978A5DA6EB953BED180496C8EBB34CFC9BE7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3396" yWindow="2388" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alza" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
@@ -697,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
@@ -854,7 +854,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>